<commit_message>
Fixed fulladder and halfadder content +problem
</commit_message>
<xml_diff>
--- a/Probleme.xlsx
+++ b/Probleme.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mar3t\Desktop\Projekt\Error_NameNotFound\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Error_NameNotFound\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF308FD-97BA-4834-BFFE-D3045F4AF28B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27750" yWindow="32280" windowWidth="27870" windowHeight="16440" xr2:uid="{C6A9F756-C385-4917-97DF-88EC24177CE1}"/>
+    <workbookView xWindow="-27750" yWindow="32280" windowWidth="27870" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Was ist das problem</t>
   </si>
@@ -48,21 +47,6 @@
     <t>Fehlermeldung</t>
   </si>
   <si>
-    <t>bsp</t>
-  </si>
-  <si>
-    <t>And.xaml.cs</t>
-  </si>
-  <si>
-    <t>And auf canvas ziehen und auf i0 von diesem klicken</t>
-  </si>
-  <si>
-    <t>Error index out of range</t>
-  </si>
-  <si>
-    <t>wenn button input 0 an and geklickt wird schmiert das program ab</t>
-  </si>
-  <si>
     <t>wenn logicbutton element geklickt wird und das peview noch nicht generiert ist teleportiert es sich zum letzten bewegtem objekt</t>
   </si>
   <si>
@@ -85,12 +69,15 @@
   </si>
   <si>
     <t>System.Runtime.CompilerServices.RuntimeWrappedException</t>
+  </si>
+  <si>
+    <t>When connecting a line to a line it goes to the top left (some times Connects with an empty input)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,7 +111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,14 +422,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFBC58C-B537-46C4-B0BF-D057383452B7}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" bestFit="1" customWidth="1"/>
@@ -453,7 +440,7 @@
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -470,64 +457,61 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>360</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>360</v>
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>